<commit_message>
EPBDS-9495 EPBDS-9497 Allow implicit cast if alias datatype values are fully included to other alias datatype. Allow explicit casts if alias datatypes has at least one value that is presented in both. Backward compatibility fix.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9497_AliasDatatypesCasts.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9497_AliasDatatypesCasts.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\explicitCastTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-9497_AliasDatatypesCasts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A15C862-7684-4F58-AB69-1865CA0EE2EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDBF64F-3063-41C8-B481-342C1FF7B855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3308" yWindow="3308" windowWidth="21600" windowHeight="11535" xr2:uid="{DDED059D-9BE1-49B6-A649-7FB85269A9F0}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="93">
   <si>
     <t>aaa</t>
   </si>
@@ -255,15 +255,6 @@
     <t>=myMethod4(field6)</t>
   </si>
   <si>
-    <t>myObj.field7</t>
-  </si>
-  <si>
-    <t>myObj.field8</t>
-  </si>
-  <si>
-    <t>myObj.field9</t>
-  </si>
-  <si>
     <t>myObj.field4</t>
   </si>
   <si>
@@ -301,17 +292,34 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>Step13</t>
+  </si>
+  <si>
+    <t>Step14</t>
+  </si>
+  <si>
+    <t>= (Datatype4) 1</t>
+  </si>
+  <si>
+    <t>= (Datatype4[]) $Step13</t>
+  </si>
+  <si>
+    <t>= (Datatype5[]) $Step13</t>
+  </si>
+  <si>
+    <t>Step15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -341,7 +349,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -660,16 +668,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CAE0D4-4D0A-4A7C-8225-83CC9680A895}">
-  <dimension ref="C3:AB35"/>
+  <dimension ref="C3:AB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12:AB14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:28" x14ac:dyDescent="0.45">
@@ -837,31 +845,31 @@
         <v>41</v>
       </c>
       <c r="T12" t="s">
+        <v>74</v>
+      </c>
+      <c r="U12" t="s">
+        <v>75</v>
+      </c>
+      <c r="V12" t="s">
+        <v>76</v>
+      </c>
+      <c r="W12" t="s">
         <v>77</v>
       </c>
-      <c r="U12" t="s">
+      <c r="X12" t="s">
         <v>78</v>
       </c>
-      <c r="V12" t="s">
+      <c r="Y12" t="s">
         <v>79</v>
       </c>
-      <c r="W12" t="s">
+      <c r="Z12" t="s">
         <v>80</v>
       </c>
-      <c r="X12" t="s">
+      <c r="AA12" t="s">
         <v>81</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="AB12" t="s">
         <v>82</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="13" spans="3:28" x14ac:dyDescent="0.45">
@@ -899,31 +907,31 @@
         <v>41</v>
       </c>
       <c r="T13" t="s">
+        <v>74</v>
+      </c>
+      <c r="U13" t="s">
+        <v>75</v>
+      </c>
+      <c r="V13" t="s">
+        <v>76</v>
+      </c>
+      <c r="W13" t="s">
         <v>77</v>
       </c>
-      <c r="U13" t="s">
+      <c r="X13" t="s">
         <v>78</v>
       </c>
-      <c r="V13" t="s">
+      <c r="Y13" t="s">
         <v>79</v>
       </c>
-      <c r="W13" t="s">
+      <c r="Z13" t="s">
         <v>80</v>
       </c>
-      <c r="X13" t="s">
+      <c r="AA13" t="s">
         <v>81</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="AB13" t="s">
         <v>82</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.45">
@@ -961,31 +969,31 @@
         <v>7</v>
       </c>
       <c r="T14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="U14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="V14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="W14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="X14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="Y14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="Z14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="AA14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="AB14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="3:28" x14ac:dyDescent="0.45">
@@ -1069,61 +1077,82 @@
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D25" s="1"/>
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D26" s="1"/>
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D27" s="1"/>
+      <c r="C27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C28" t="s">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C30" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="H28" t="s">
+      <c r="D30" s="1"/>
+      <c r="H30" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="H29" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="H31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C33" t="s">
         <v>35</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H33" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C32" t="s">
-        <v>20</v>
-      </c>
-      <c r="H32" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C36" t="s">
         <v>42</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H36" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C35" t="s">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C37" t="s">
         <v>37</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H37" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>